<commit_message>
added some table summary results
</commit_message>
<xml_diff>
--- a/Python/output/synthetic/FAresults-cutsharing.xlsx
+++ b/Python/output/synthetic/FAresults-cutsharing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongjis/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/output/synthetic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B4485B2-03E3-3A43-9C6E-33DE088E5F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C1DA02F5-DB4A-A04B-ACB9-43EFE5861F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15800" yWindow="5200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{F4B921D5-876A-DB47-B723-44565D89F8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="FAresults-cutsharing" sheetId="1" r:id="rId1"/>
@@ -73,26 +73,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -100,7 +100,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -108,7 +108,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -116,35 +116,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,7 +152,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,14 +160,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -175,14 +175,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,7 +190,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -198,14 +198,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -622,39 +622,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -706,7 +706,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -817,13 +817,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -832,6 +825,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -896,28 +896,45 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4C9ADF-43A8-C840-954A-44FCF844F852}">
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1901,22 +1918,22 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1838.1298495297101</v>
+        <v>1838.12985</v>
       </c>
       <c r="L22">
         <v>14425</v>
       </c>
       <c r="M22">
-        <v>65326.3626451487</v>
+        <v>65326.362650000003</v>
       </c>
       <c r="N22">
-        <v>7000.5981005990998</v>
+        <v>7000.5981009999996</v>
       </c>
       <c r="O22">
-        <v>799.65979599952698</v>
+        <v>799.65979600000003</v>
       </c>
       <c r="P22">
-        <v>0.54915618896484297</v>
+        <v>0.54915618899999996</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
@@ -1951,22 +1968,1722 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <v>1866.22240496975</v>
+        <v>1866.222405</v>
       </c>
       <c r="L23">
         <v>1319</v>
       </c>
       <c r="M23">
-        <v>65348.583695225097</v>
+        <v>65348.583700000003</v>
       </c>
       <c r="N23">
-        <v>7003.6638287376099</v>
+        <v>7003.6638290000001</v>
       </c>
       <c r="O23">
-        <v>411.974531888961</v>
+        <v>411.97453189999999</v>
       </c>
       <c r="P23">
-        <v>1.64447617530822</v>
+        <v>1.6444761750000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>57</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>2936.6182560000002</v>
+      </c>
+      <c r="L24">
+        <v>11273</v>
+      </c>
+      <c r="M24">
+        <v>68069.381359999999</v>
+      </c>
+      <c r="N24">
+        <v>7181.5407789999999</v>
+      </c>
+      <c r="O24">
+        <v>636.90328190000002</v>
+      </c>
+      <c r="P24">
+        <v>0.55519795400000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>57</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>0.5</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>3003.95496</v>
+      </c>
+      <c r="L25">
+        <v>1346</v>
+      </c>
+      <c r="M25">
+        <v>68721.671870000006</v>
+      </c>
+      <c r="N25">
+        <v>7186.335986</v>
+      </c>
+      <c r="O25">
+        <v>329.13315080000001</v>
+      </c>
+      <c r="P25">
+        <v>1.1649761199999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>57</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>5847.1416570000001</v>
+      </c>
+      <c r="L26">
+        <v>15253</v>
+      </c>
+      <c r="M26">
+        <v>74913.144469999999</v>
+      </c>
+      <c r="N26">
+        <v>7579.9912729999996</v>
+      </c>
+      <c r="O26">
+        <v>886.83198830000003</v>
+      </c>
+      <c r="P26">
+        <v>0.57710099199999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>57</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>5949.6770450000004</v>
+      </c>
+      <c r="L27">
+        <v>1064</v>
+      </c>
+      <c r="M27">
+        <v>81450.097559999995</v>
+      </c>
+      <c r="N27">
+        <v>7784.2198440000002</v>
+      </c>
+      <c r="O27">
+        <v>250.36078789999999</v>
+      </c>
+      <c r="P27">
+        <v>1.0227770810000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>57</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>3339.0862244623199</v>
+      </c>
+      <c r="L28">
+        <v>16526</v>
+      </c>
+      <c r="M28">
+        <v>130710.226791803</v>
+      </c>
+      <c r="N28">
+        <v>13487.372990363499</v>
+      </c>
+      <c r="O28">
+        <v>1039.2628529071801</v>
+      </c>
+      <c r="P28">
+        <v>0.62824487686157204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>3378.59243179654</v>
+      </c>
+      <c r="L29">
+        <v>1060</v>
+      </c>
+      <c r="M29">
+        <v>130714.64745188699</v>
+      </c>
+      <c r="N29">
+        <v>13487.9944975831</v>
+      </c>
+      <c r="O29">
+        <v>246.765195131301</v>
+      </c>
+      <c r="P29">
+        <v>1.09134101867675</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>57</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>20</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>5454.964696</v>
+      </c>
+      <c r="L30">
+        <v>15004</v>
+      </c>
+      <c r="M30">
+        <v>136545.11199999999</v>
+      </c>
+      <c r="N30">
+        <v>13850.97099</v>
+      </c>
+      <c r="O30">
+        <v>1057.6004029999999</v>
+      </c>
+      <c r="P30">
+        <v>0.72658705700000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>57</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>20</v>
+      </c>
+      <c r="H31">
+        <v>0.5</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>5519.4289330000001</v>
+      </c>
+      <c r="L31">
+        <v>834</v>
+      </c>
+      <c r="M31">
+        <v>137549.4252</v>
+      </c>
+      <c r="N31">
+        <v>13852.37262</v>
+      </c>
+      <c r="O31">
+        <v>189.37044309999999</v>
+      </c>
+      <c r="P31">
+        <v>0.68263792999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>57</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>20</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>11032.75325</v>
+      </c>
+      <c r="L32">
+        <v>11646</v>
+      </c>
+      <c r="M32">
+        <v>150679.47839999999</v>
+      </c>
+      <c r="N32">
+        <v>14632.796829999999</v>
+      </c>
+      <c r="O32">
+        <v>809.09585519999996</v>
+      </c>
+      <c r="P32">
+        <v>0.99220109000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>57</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>20</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>11318.36217</v>
+      </c>
+      <c r="L33">
+        <v>785</v>
+      </c>
+      <c r="M33">
+        <v>162062.2524</v>
+      </c>
+      <c r="N33">
+        <v>15021.633620000001</v>
+      </c>
+      <c r="O33">
+        <v>183.32869890000001</v>
+      </c>
+      <c r="P33">
+        <v>0.77987885499999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>57</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>30</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>5175.8750179999997</v>
+      </c>
+      <c r="L34">
+        <v>13566</v>
+      </c>
+      <c r="M34">
+        <v>195821.91099999999</v>
+      </c>
+      <c r="N34">
+        <v>19976.407800000001</v>
+      </c>
+      <c r="O34">
+        <v>997.10074280000003</v>
+      </c>
+      <c r="P34">
+        <v>1.154596806</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>57</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>30</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>5255.1838189999999</v>
+      </c>
+      <c r="L35">
+        <v>1011</v>
+      </c>
+      <c r="M35">
+        <v>195870.0215</v>
+      </c>
+      <c r="N35">
+        <v>19986.939729999998</v>
+      </c>
+      <c r="O35">
+        <v>242.02219769999999</v>
+      </c>
+      <c r="P35">
+        <v>0.81650471700000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>30</v>
+      </c>
+      <c r="H36">
+        <v>0.5</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>8368.2806550000005</v>
+      </c>
+      <c r="L36">
+        <v>14165</v>
+      </c>
+      <c r="M36">
+        <v>204352.4866</v>
+      </c>
+      <c r="N36">
+        <v>20593.657060000001</v>
+      </c>
+      <c r="O36">
+        <v>1131.0296900000001</v>
+      </c>
+      <c r="P36">
+        <v>1.6769528389999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>57</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>30</v>
+      </c>
+      <c r="H37">
+        <v>0.5</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>8454.5544699999991</v>
+      </c>
+      <c r="L37">
+        <v>1547</v>
+      </c>
+      <c r="M37">
+        <v>206047.26120000001</v>
+      </c>
+      <c r="N37">
+        <v>20576.47697</v>
+      </c>
+      <c r="O37">
+        <v>428.30962899999997</v>
+      </c>
+      <c r="P37">
+        <v>0.91889595999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>57</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>30</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>16747.094260000002</v>
+      </c>
+      <c r="L38">
+        <v>21431</v>
+      </c>
+      <c r="M38">
+        <v>226062.17939999999</v>
+      </c>
+      <c r="N38">
+        <v>21884.979240000001</v>
+      </c>
+      <c r="O38">
+        <v>1778.1165189999999</v>
+      </c>
+      <c r="P38">
+        <v>1.345211744</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>57</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>30</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>16899.02506</v>
+      </c>
+      <c r="L39">
+        <v>1131</v>
+      </c>
+      <c r="M39">
+        <v>244016.93119999999</v>
+      </c>
+      <c r="N39">
+        <v>22467.056809999998</v>
+      </c>
+      <c r="O39">
+        <v>293.83375189999998</v>
+      </c>
+      <c r="P39">
+        <v>0.61452317199999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>57</v>
+      </c>
+      <c r="F40">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1776.21498</v>
+      </c>
+      <c r="L40">
+        <v>12548</v>
+      </c>
+      <c r="M40">
+        <v>65342.28944</v>
+      </c>
+      <c r="N40">
+        <v>7005.2295860000004</v>
+      </c>
+      <c r="O40">
+        <v>816.08924009999998</v>
+      </c>
+      <c r="P40">
+        <v>1.1335918899999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>57</v>
+      </c>
+      <c r="F41">
+        <v>9</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1808.513066</v>
+      </c>
+      <c r="L41">
+        <v>1016</v>
+      </c>
+      <c r="M41">
+        <v>65349.236320000004</v>
+      </c>
+      <c r="N41">
+        <v>7006.2968170000004</v>
+      </c>
+      <c r="O41">
+        <v>298.55551100000002</v>
+      </c>
+      <c r="P41">
+        <v>0.71214222900000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>57</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>10</v>
+      </c>
+      <c r="H42">
+        <v>0.5</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>2952.7039799999998</v>
+      </c>
+      <c r="L42">
+        <v>16266</v>
+      </c>
+      <c r="M42">
+        <v>68160.411070000002</v>
+      </c>
+      <c r="N42">
+        <v>7192.6782059999996</v>
+      </c>
+      <c r="O42">
+        <v>1182.4377260000001</v>
+      </c>
+      <c r="P42">
+        <v>1.5713529589999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>57</v>
+      </c>
+      <c r="F43">
+        <v>9</v>
+      </c>
+      <c r="G43">
+        <v>10</v>
+      </c>
+      <c r="H43">
+        <v>0.5</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>2979.5718010000001</v>
+      </c>
+      <c r="L43">
+        <v>1657</v>
+      </c>
+      <c r="M43">
+        <v>68651.480410000004</v>
+      </c>
+      <c r="N43">
+        <v>7192.5016089999999</v>
+      </c>
+      <c r="O43">
+        <v>537.31948179999995</v>
+      </c>
+      <c r="P43">
+        <v>0.69591784499999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>57</v>
+      </c>
+      <c r="F44">
+        <v>9</v>
+      </c>
+      <c r="G44">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>5917.7665340000003</v>
+      </c>
+      <c r="L44">
+        <v>16253</v>
+      </c>
+      <c r="M44">
+        <v>74834.947480000003</v>
+      </c>
+      <c r="N44">
+        <v>7569.6149649999998</v>
+      </c>
+      <c r="O44">
+        <v>1209.0373039999999</v>
+      </c>
+      <c r="P44">
+        <v>1.105711699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>57</v>
+      </c>
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>10</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>6017.4192720000001</v>
+      </c>
+      <c r="L45">
+        <v>800</v>
+      </c>
+      <c r="M45">
+        <v>81024.082689999996</v>
+      </c>
+      <c r="N45">
+        <v>7740.0884219999998</v>
+      </c>
+      <c r="O45">
+        <v>228.08957599999999</v>
+      </c>
+      <c r="P45">
+        <v>0.74306726499999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>57</v>
+      </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>20</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>3317.8923159999999</v>
+      </c>
+      <c r="L46">
+        <v>15163</v>
+      </c>
+      <c r="M46">
+        <v>130719.91929999999</v>
+      </c>
+      <c r="N46">
+        <v>13488.16697</v>
+      </c>
+      <c r="O46">
+        <v>1184.6953450000001</v>
+      </c>
+      <c r="P46">
+        <v>2.1333391669999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>57</v>
+      </c>
+      <c r="F47">
+        <v>9</v>
+      </c>
+      <c r="G47">
+        <v>20</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>3359.0684670000001</v>
+      </c>
+      <c r="L47">
+        <v>1805</v>
+      </c>
+      <c r="M47">
+        <v>130739.86500000001</v>
+      </c>
+      <c r="N47">
+        <v>13491.636039999999</v>
+      </c>
+      <c r="O47">
+        <v>616.44342710000001</v>
+      </c>
+      <c r="P47">
+        <v>0.86595892900000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>57</v>
+      </c>
+      <c r="F48">
+        <v>9</v>
+      </c>
+      <c r="G48">
+        <v>20</v>
+      </c>
+      <c r="H48">
+        <v>0.5</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>5481.559929</v>
+      </c>
+      <c r="L48">
+        <v>16858</v>
+      </c>
+      <c r="M48">
+        <v>136453.45610000001</v>
+      </c>
+      <c r="N48">
+        <v>13858.19364</v>
+      </c>
+      <c r="O48">
+        <v>1486.3668580000001</v>
+      </c>
+      <c r="P48">
+        <v>1.70206809</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>57</v>
+      </c>
+      <c r="F49">
+        <v>9</v>
+      </c>
+      <c r="G49">
+        <v>20</v>
+      </c>
+      <c r="H49">
+        <v>0.5</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>5537.6078559999996</v>
+      </c>
+      <c r="L49">
+        <v>1564</v>
+      </c>
+      <c r="M49">
+        <v>137577.81630000001</v>
+      </c>
+      <c r="N49">
+        <v>13857.57043</v>
+      </c>
+      <c r="O49">
+        <v>524.87840600000004</v>
+      </c>
+      <c r="P49">
+        <v>0.85755085900000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>57</v>
+      </c>
+      <c r="F50">
+        <v>9</v>
+      </c>
+      <c r="G50">
+        <v>20</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>11188.234200000001</v>
+      </c>
+      <c r="L50">
+        <v>17736</v>
+      </c>
+      <c r="M50">
+        <v>149407.81049999999</v>
+      </c>
+      <c r="N50">
+        <v>14592.51204</v>
+      </c>
+      <c r="O50">
+        <v>1594.4718700000001</v>
+      </c>
+      <c r="P50">
+        <v>1.2926788330000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>57</v>
+      </c>
+      <c r="F51">
+        <v>9</v>
+      </c>
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>11419.01821</v>
+      </c>
+      <c r="L51">
+        <v>928</v>
+      </c>
+      <c r="M51">
+        <v>162225.24530000001</v>
+      </c>
+      <c r="N51">
+        <v>15050.10052</v>
+      </c>
+      <c r="O51">
+        <v>288.58421709999999</v>
+      </c>
+      <c r="P51">
+        <v>0.87529396999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>57</v>
+      </c>
+      <c r="F52">
+        <v>9</v>
+      </c>
+      <c r="G52">
+        <v>30</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>5122.3782499999998</v>
+      </c>
+      <c r="L52">
+        <v>14785</v>
+      </c>
+      <c r="M52">
+        <v>195882.1219</v>
+      </c>
+      <c r="N52">
+        <v>19987.115010000001</v>
+      </c>
+      <c r="O52">
+        <v>1378.5944460000001</v>
+      </c>
+      <c r="P52">
+        <v>1.5020091529999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>57</v>
+      </c>
+      <c r="F53">
+        <v>9</v>
+      </c>
+      <c r="G53">
+        <v>30</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>5187.3580190000002</v>
+      </c>
+      <c r="L53">
+        <v>1084</v>
+      </c>
+      <c r="M53">
+        <v>195909.42310000001</v>
+      </c>
+      <c r="N53">
+        <v>19994.732749999999</v>
+      </c>
+      <c r="O53">
+        <v>354.76902130000002</v>
+      </c>
+      <c r="P53">
+        <v>1.013789177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>57</v>
+      </c>
+      <c r="F54">
+        <v>9</v>
+      </c>
+      <c r="G54">
+        <v>30</v>
+      </c>
+      <c r="H54">
+        <v>0.5</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>8385.2995059999994</v>
+      </c>
+      <c r="L54">
+        <v>16019</v>
+      </c>
+      <c r="M54">
+        <v>204606.02910000001</v>
+      </c>
+      <c r="N54">
+        <v>20593.942159999999</v>
+      </c>
+      <c r="O54">
+        <v>1598.6790699999999</v>
+      </c>
+      <c r="P54">
+        <v>1.260969877</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>57</v>
+      </c>
+      <c r="F55">
+        <v>9</v>
+      </c>
+      <c r="G55">
+        <v>30</v>
+      </c>
+      <c r="H55">
+        <v>0.5</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>8456.4576969999998</v>
+      </c>
+      <c r="L55">
+        <v>740</v>
+      </c>
+      <c r="M55">
+        <v>207284.72839999999</v>
+      </c>
+      <c r="N55">
+        <v>20582.905890000002</v>
+      </c>
+      <c r="O55">
+        <v>222.16919490000001</v>
+      </c>
+      <c r="P55">
+        <v>1.024814844</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>57</v>
+      </c>
+      <c r="F56">
+        <v>9</v>
+      </c>
+      <c r="G56">
+        <v>30</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>16618.068759999998</v>
+      </c>
+      <c r="L56">
+        <v>16166</v>
+      </c>
+      <c r="M56">
+        <v>225354.9203</v>
+      </c>
+      <c r="N56">
+        <v>21777.106540000001</v>
+      </c>
+      <c r="O56">
+        <v>1740.7936010000001</v>
+      </c>
+      <c r="P56">
+        <v>1.6466450690000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>57</v>
+      </c>
+      <c r="F57">
+        <v>9</v>
+      </c>
+      <c r="G57">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>16986.258450000001</v>
+      </c>
+      <c r="L57">
+        <v>1154</v>
+      </c>
+      <c r="M57">
+        <v>243460.78630000001</v>
+      </c>
+      <c r="N57">
+        <v>22411.01772</v>
+      </c>
+      <c r="O57">
+        <v>396.14589999999998</v>
+      </c>
+      <c r="P57">
+        <v>1.6466450690000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>